<commit_message>
LipnoV2 TOPOLOGIE DONE 24.2.15:21
</commit_message>
<xml_diff>
--- a/hodiny.xlsx
+++ b/hodiny.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68966F98-143F-402F-9BA3-B339F694A6E4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C55C3E9-9E16-4F4A-A66B-F98B64AD3528}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="98">
   <si>
     <t>Vektorizace, první sada</t>
   </si>
@@ -825,9 +825,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -842,6 +839,9 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1184,7 +1184,7 @@
   <dimension ref="A1:X342"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A235" workbookViewId="0">
-      <selection activeCell="K260" sqref="K260"/>
+      <selection activeCell="L259" sqref="L259"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1206,10 +1206,10 @@
       <c r="B1" s="51"/>
       <c r="C1" s="11"/>
       <c r="D1" s="11"/>
-      <c r="E1" s="68" t="s">
+      <c r="E1" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="69" t="s">
+      <c r="F1" s="68" t="s">
         <v>18</v>
       </c>
       <c r="G1" s="17" t="s">
@@ -1230,8 +1230,8 @@
       <c r="D2" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="68"/>
-      <c r="F2" s="69"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="68"/>
       <c r="G2" s="12" t="s">
         <v>14</v>
       </c>
@@ -1411,7 +1411,7 @@
         <v>16716.666666666664</v>
       </c>
       <c r="J13" s="6"/>
-      <c r="K13" s="66"/>
+      <c r="K13" s="71"/>
       <c r="L13" s="8"/>
       <c r="M13" s="8"/>
       <c r="N13" s="9"/>
@@ -1427,7 +1427,7 @@
       <c r="X13" s="6"/>
     </row>
     <row r="14" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B14" s="67" t="s">
+      <c r="B14" s="66" t="s">
         <v>10</v>
       </c>
       <c r="C14" s="4">
@@ -1457,7 +1457,7 @@
         <v>16915</v>
       </c>
       <c r="J14" s="6"/>
-      <c r="K14" s="66"/>
+      <c r="K14" s="71"/>
       <c r="L14" s="8"/>
       <c r="M14" s="8"/>
       <c r="N14" s="9"/>
@@ -1473,7 +1473,7 @@
       <c r="X14" s="6"/>
     </row>
     <row r="15" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B15" s="67"/>
+      <c r="B15" s="66"/>
       <c r="C15" s="4">
         <v>0.68402777777777779</v>
       </c>
@@ -1501,7 +1501,7 @@
         <v>17184.166666666664</v>
       </c>
       <c r="J15" s="6"/>
-      <c r="K15" s="66"/>
+      <c r="K15" s="71"/>
       <c r="L15" s="8"/>
       <c r="M15" s="8"/>
       <c r="N15" s="9"/>
@@ -1517,7 +1517,7 @@
       <c r="X15" s="6"/>
     </row>
     <row r="16" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B16" s="67"/>
+      <c r="B16" s="66"/>
       <c r="C16" s="4">
         <v>0.76041666666666663</v>
       </c>
@@ -1545,7 +1545,7 @@
         <v>17269.166666666664</v>
       </c>
       <c r="J16" s="6"/>
-      <c r="K16" s="66"/>
+      <c r="K16" s="71"/>
       <c r="L16" s="8"/>
       <c r="M16" s="8"/>
       <c r="N16" s="9"/>
@@ -1561,7 +1561,7 @@
       <c r="X16" s="6"/>
     </row>
     <row r="17" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B17" s="67"/>
+      <c r="B17" s="66"/>
       <c r="C17" s="4">
         <v>0.80208333333333337</v>
       </c>
@@ -1589,7 +1589,7 @@
         <v>17524.166666666664</v>
       </c>
       <c r="J17" s="6"/>
-      <c r="K17" s="66"/>
+      <c r="K17" s="71"/>
       <c r="L17" s="8"/>
       <c r="M17" s="8"/>
       <c r="N17" s="9"/>
@@ -1605,7 +1605,7 @@
       <c r="X17" s="6"/>
     </row>
     <row r="18" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B18" s="67"/>
+      <c r="B18" s="66"/>
       <c r="C18" s="4">
         <v>0.875</v>
       </c>
@@ -1633,7 +1633,7 @@
         <v>17651.666666666664</v>
       </c>
       <c r="J18" s="6"/>
-      <c r="K18" s="66"/>
+      <c r="K18" s="71"/>
       <c r="L18" s="8"/>
       <c r="M18" s="8"/>
       <c r="N18" s="9"/>
@@ -1649,7 +1649,7 @@
       <c r="X18" s="6"/>
     </row>
     <row r="19" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B19" s="67" t="s">
+      <c r="B19" s="66" t="s">
         <v>11</v>
       </c>
       <c r="C19" s="4">
@@ -1679,7 +1679,7 @@
         <v>17878.333333333332</v>
       </c>
       <c r="J19" s="6"/>
-      <c r="K19" s="66"/>
+      <c r="K19" s="71"/>
       <c r="L19" s="8"/>
       <c r="M19" s="8"/>
       <c r="N19" s="9"/>
@@ -1695,7 +1695,7 @@
       <c r="X19" s="6"/>
     </row>
     <row r="20" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B20" s="67"/>
+      <c r="B20" s="66"/>
       <c r="C20" s="4">
         <v>0.59722222222222221</v>
       </c>
@@ -1723,7 +1723,7 @@
         <v>18246.666666666664</v>
       </c>
       <c r="J20" s="6"/>
-      <c r="K20" s="66"/>
+      <c r="K20" s="71"/>
       <c r="L20" s="8"/>
       <c r="M20" s="8"/>
       <c r="N20" s="9"/>
@@ -1739,7 +1739,7 @@
       <c r="X20" s="6"/>
     </row>
     <row r="21" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B21" s="67"/>
+      <c r="B21" s="66"/>
       <c r="C21" s="4">
         <v>0.69444444444444453</v>
       </c>
@@ -1767,7 +1767,7 @@
         <v>18388.333333333332</v>
       </c>
       <c r="J21" s="6"/>
-      <c r="K21" s="66"/>
+      <c r="K21" s="71"/>
       <c r="L21" s="8"/>
       <c r="M21" s="8"/>
       <c r="N21" s="9"/>
@@ -1783,7 +1783,7 @@
       <c r="X21" s="6"/>
     </row>
     <row r="22" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B22" s="67"/>
+      <c r="B22" s="66"/>
       <c r="C22" s="4">
         <v>0.75</v>
       </c>
@@ -1811,7 +1811,7 @@
         <v>18515.833333333332</v>
       </c>
       <c r="J22" s="6"/>
-      <c r="K22" s="66"/>
+      <c r="K22" s="71"/>
       <c r="L22" s="8"/>
       <c r="M22" s="8"/>
       <c r="N22" s="9"/>
@@ -1827,7 +1827,7 @@
       <c r="X22" s="6"/>
     </row>
     <row r="23" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B23" s="67"/>
+      <c r="B23" s="66"/>
       <c r="C23" s="4">
         <v>0.79513888888888884</v>
       </c>
@@ -1871,7 +1871,7 @@
       <c r="X23" s="6"/>
     </row>
     <row r="24" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B24" s="71" t="s">
+      <c r="B24" s="70" t="s">
         <v>12</v>
       </c>
       <c r="C24" s="4">
@@ -1917,7 +1917,7 @@
       <c r="X24" s="6"/>
     </row>
     <row r="25" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B25" s="71"/>
+      <c r="B25" s="70"/>
       <c r="C25" s="4">
         <v>0.58333333333333337</v>
       </c>
@@ -1961,7 +1961,7 @@
       <c r="X25" s="6"/>
     </row>
     <row r="26" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B26" s="71"/>
+      <c r="B26" s="70"/>
       <c r="C26" s="4">
         <v>0.69444444444444453</v>
       </c>
@@ -2005,7 +2005,7 @@
       <c r="X26" s="6"/>
     </row>
     <row r="27" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B27" s="71"/>
+      <c r="B27" s="70"/>
       <c r="C27" s="4">
         <v>0.83333333333333337</v>
       </c>
@@ -2049,7 +2049,7 @@
       <c r="X27" s="6"/>
     </row>
     <row r="28" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B28" s="67" t="s">
+      <c r="B28" s="66" t="s">
         <v>19</v>
       </c>
       <c r="C28" s="4">
@@ -2095,7 +2095,7 @@
       <c r="X28" s="6"/>
     </row>
     <row r="29" spans="2:24" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="70"/>
+      <c r="B29" s="69"/>
       <c r="C29" s="27">
         <v>0.61111111111111105</v>
       </c>
@@ -2140,10 +2140,10 @@
       <c r="B31" s="51"/>
       <c r="C31" s="11"/>
       <c r="D31" s="11"/>
-      <c r="E31" s="68" t="s">
+      <c r="E31" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="F31" s="69" t="s">
+      <c r="F31" s="68" t="s">
         <v>18</v>
       </c>
       <c r="G31" s="17" t="s">
@@ -2164,8 +2164,8 @@
       <c r="D32" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E32" s="68"/>
-      <c r="F32" s="69"/>
+      <c r="E32" s="67"/>
+      <c r="F32" s="68"/>
       <c r="G32" s="12" t="s">
         <v>14</v>
       </c>
@@ -2180,7 +2180,7 @@
       </c>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B33" s="67" t="s">
+      <c r="B33" s="66" t="s">
         <v>21</v>
       </c>
       <c r="C33" s="24">
@@ -2211,7 +2211,7 @@
       </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B34" s="67"/>
+      <c r="B34" s="66"/>
       <c r="C34" s="4">
         <v>0.65277777777777779</v>
       </c>
@@ -2240,7 +2240,7 @@
       </c>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B35" s="67"/>
+      <c r="B35" s="66"/>
       <c r="C35" s="4">
         <v>0.67013888888888884</v>
       </c>
@@ -2300,7 +2300,7 @@
       </c>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B37" s="67" t="s">
+      <c r="B37" s="66" t="s">
         <v>24</v>
       </c>
       <c r="C37" s="4">
@@ -2331,7 +2331,7 @@
       </c>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B38" s="67"/>
+      <c r="B38" s="66"/>
       <c r="C38" s="4">
         <v>0.77083333333333337</v>
       </c>
@@ -2360,7 +2360,7 @@
       </c>
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B39" s="67"/>
+      <c r="B39" s="66"/>
       <c r="C39" s="4">
         <v>0.77777777777777779</v>
       </c>
@@ -2389,7 +2389,7 @@
       </c>
     </row>
     <row r="40" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B40" s="67"/>
+      <c r="B40" s="66"/>
       <c r="C40" s="4">
         <v>0.93055555555555547</v>
       </c>
@@ -2418,7 +2418,7 @@
       </c>
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B41" s="67" t="s">
+      <c r="B41" s="66" t="s">
         <v>25</v>
       </c>
       <c r="C41" s="4">
@@ -2449,7 +2449,7 @@
       </c>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B42" s="67"/>
+      <c r="B42" s="66"/>
       <c r="C42" s="4">
         <v>5.2083333333333336E-2</v>
       </c>
@@ -2478,7 +2478,7 @@
       </c>
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B43" s="67"/>
+      <c r="B43" s="66"/>
       <c r="C43" s="4">
         <v>0.60069444444444442</v>
       </c>
@@ -2507,7 +2507,7 @@
       </c>
     </row>
     <row r="44" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B44" s="67"/>
+      <c r="B44" s="66"/>
       <c r="C44" s="4">
         <v>0.70138888888888884</v>
       </c>
@@ -2536,7 +2536,7 @@
       </c>
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B45" s="67"/>
+      <c r="B45" s="66"/>
       <c r="C45" s="4">
         <v>0.78472222222222221</v>
       </c>
@@ -2565,7 +2565,7 @@
       </c>
     </row>
     <row r="46" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B46" s="67"/>
+      <c r="B46" s="66"/>
       <c r="C46" s="4">
         <v>0.92708333333333337</v>
       </c>
@@ -2594,7 +2594,7 @@
       </c>
     </row>
     <row r="47" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B47" s="67" t="s">
+      <c r="B47" s="66" t="s">
         <v>26</v>
       </c>
       <c r="C47" s="4">
@@ -2625,7 +2625,7 @@
       </c>
     </row>
     <row r="48" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B48" s="67"/>
+      <c r="B48" s="66"/>
       <c r="C48" s="4">
         <v>0.63541666666666663</v>
       </c>
@@ -2654,7 +2654,7 @@
       </c>
     </row>
     <row r="49" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B49" s="67"/>
+      <c r="B49" s="66"/>
       <c r="C49" s="4">
         <v>0.74305555555555547</v>
       </c>
@@ -2683,7 +2683,7 @@
       </c>
     </row>
     <row r="50" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B50" s="67"/>
+      <c r="B50" s="66"/>
       <c r="C50" s="4">
         <v>0.78819444444444453</v>
       </c>
@@ -2712,7 +2712,7 @@
       </c>
     </row>
     <row r="51" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B51" s="67"/>
+      <c r="B51" s="66"/>
       <c r="C51" s="4">
         <v>0.81597222222222221</v>
       </c>
@@ -2741,7 +2741,7 @@
       </c>
     </row>
     <row r="52" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B52" s="67"/>
+      <c r="B52" s="66"/>
       <c r="C52" s="4">
         <v>0.89583333333333337</v>
       </c>
@@ -2773,7 +2773,7 @@
       </c>
     </row>
     <row r="53" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B53" s="67"/>
+      <c r="B53" s="66"/>
       <c r="C53" s="4">
         <v>0.99652777777777779</v>
       </c>
@@ -2805,7 +2805,7 @@
       </c>
     </row>
     <row r="54" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B54" s="67" t="s">
+      <c r="B54" s="66" t="s">
         <v>30</v>
       </c>
       <c r="C54" s="4">
@@ -2839,7 +2839,7 @@
       </c>
     </row>
     <row r="55" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B55" s="67"/>
+      <c r="B55" s="66"/>
       <c r="C55" s="4">
         <v>0.19444444444444445</v>
       </c>
@@ -2868,7 +2868,7 @@
       </c>
     </row>
     <row r="56" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B56" s="67"/>
+      <c r="B56" s="66"/>
       <c r="C56" s="4">
         <v>0.625</v>
       </c>
@@ -2897,7 +2897,7 @@
       </c>
     </row>
     <row r="57" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B57" s="67"/>
+      <c r="B57" s="66"/>
       <c r="C57" s="4">
         <v>0.66666666666666663</v>
       </c>
@@ -2926,7 +2926,7 @@
       </c>
     </row>
     <row r="58" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B58" s="67"/>
+      <c r="B58" s="66"/>
       <c r="C58" s="4">
         <v>0.70138888888888884</v>
       </c>
@@ -2955,7 +2955,7 @@
       </c>
     </row>
     <row r="59" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B59" s="67"/>
+      <c r="B59" s="66"/>
       <c r="C59" s="4">
         <v>0.72916666666666663</v>
       </c>
@@ -3015,7 +3015,7 @@
       </c>
     </row>
     <row r="61" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B61" s="67" t="s">
+      <c r="B61" s="66" t="s">
         <v>32</v>
       </c>
       <c r="C61" s="4">
@@ -3046,7 +3046,7 @@
       </c>
     </row>
     <row r="62" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B62" s="67"/>
+      <c r="B62" s="66"/>
       <c r="C62" s="4">
         <v>0.77083333333333337</v>
       </c>
@@ -3075,7 +3075,7 @@
       </c>
     </row>
     <row r="63" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B63" s="67" t="s">
+      <c r="B63" s="66" t="s">
         <v>33</v>
       </c>
       <c r="C63" s="4">
@@ -3106,7 +3106,7 @@
       </c>
     </row>
     <row r="64" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B64" s="67"/>
+      <c r="B64" s="66"/>
       <c r="C64" s="4">
         <v>0.86111111111111116</v>
       </c>
@@ -3135,7 +3135,7 @@
       </c>
     </row>
     <row r="65" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B65" s="67"/>
+      <c r="B65" s="66"/>
       <c r="C65" s="4">
         <v>0.88888888888888884</v>
       </c>
@@ -3164,7 +3164,7 @@
       </c>
     </row>
     <row r="66" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B66" s="67" t="s">
+      <c r="B66" s="66" t="s">
         <v>34</v>
       </c>
       <c r="C66" s="4">
@@ -3195,7 +3195,7 @@
       </c>
     </row>
     <row r="67" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B67" s="67"/>
+      <c r="B67" s="66"/>
       <c r="C67" s="4">
         <v>0.76041666666666663</v>
       </c>
@@ -3224,7 +3224,7 @@
       </c>
     </row>
     <row r="68" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B68" s="67"/>
+      <c r="B68" s="66"/>
       <c r="C68" s="4">
         <v>0.89930555555555547</v>
       </c>
@@ -3253,7 +3253,7 @@
       </c>
     </row>
     <row r="69" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B69" s="67"/>
+      <c r="B69" s="66"/>
       <c r="C69" s="4">
         <v>0.92361111111111116</v>
       </c>
@@ -3282,7 +3282,7 @@
       </c>
     </row>
     <row r="70" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B70" s="67" t="s">
+      <c r="B70" s="66" t="s">
         <v>35</v>
       </c>
       <c r="C70" s="4">
@@ -3313,7 +3313,7 @@
       </c>
     </row>
     <row r="71" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B71" s="67"/>
+      <c r="B71" s="66"/>
       <c r="C71" s="4">
         <v>0.72222222222222221</v>
       </c>
@@ -3373,7 +3373,7 @@
       </c>
     </row>
     <row r="73" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B73" s="67" t="s">
+      <c r="B73" s="66" t="s">
         <v>37</v>
       </c>
       <c r="C73" s="4">
@@ -3404,7 +3404,7 @@
       </c>
     </row>
     <row r="74" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B74" s="67"/>
+      <c r="B74" s="66"/>
       <c r="C74" s="4">
         <v>0.68055555555555547</v>
       </c>
@@ -3433,7 +3433,7 @@
       </c>
     </row>
     <row r="75" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B75" s="67" t="s">
+      <c r="B75" s="66" t="s">
         <v>38</v>
       </c>
       <c r="C75" s="4">
@@ -3464,7 +3464,7 @@
       </c>
     </row>
     <row r="76" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B76" s="67"/>
+      <c r="B76" s="66"/>
       <c r="C76" s="4">
         <v>0.68402777777777779</v>
       </c>
@@ -3493,7 +3493,7 @@
       </c>
     </row>
     <row r="77" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B77" s="67"/>
+      <c r="B77" s="66"/>
       <c r="C77" s="4">
         <v>0.79513888888888884</v>
       </c>
@@ -3522,7 +3522,7 @@
       </c>
     </row>
     <row r="78" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B78" s="67"/>
+      <c r="B78" s="66"/>
       <c r="C78" s="4">
         <v>0.96875</v>
       </c>
@@ -3551,7 +3551,7 @@
       </c>
     </row>
     <row r="79" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B79" s="67" t="s">
+      <c r="B79" s="66" t="s">
         <v>39</v>
       </c>
       <c r="C79" s="4">
@@ -3585,7 +3585,7 @@
       </c>
     </row>
     <row r="80" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B80" s="67"/>
+      <c r="B80" s="66"/>
       <c r="C80" s="4">
         <v>0.65625</v>
       </c>
@@ -3614,7 +3614,7 @@
       </c>
     </row>
     <row r="81" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B81" s="67" t="s">
+      <c r="B81" s="66" t="s">
         <v>41</v>
       </c>
       <c r="C81" s="4">
@@ -3645,7 +3645,7 @@
       </c>
     </row>
     <row r="82" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B82" s="67"/>
+      <c r="B82" s="66"/>
       <c r="C82" s="4">
         <v>0.66666666666666663</v>
       </c>
@@ -3674,7 +3674,7 @@
       </c>
     </row>
     <row r="83" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B83" s="67"/>
+      <c r="B83" s="66"/>
       <c r="C83" s="4">
         <v>0.69791666666666663</v>
       </c>
@@ -3703,7 +3703,7 @@
       </c>
     </row>
     <row r="84" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B84" s="67" t="s">
+      <c r="B84" s="66" t="s">
         <v>42</v>
       </c>
       <c r="C84" s="4">
@@ -3734,7 +3734,7 @@
       </c>
     </row>
     <row r="85" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B85" s="67"/>
+      <c r="B85" s="66"/>
       <c r="C85" s="4">
         <v>0.61805555555555558</v>
       </c>
@@ -3763,7 +3763,7 @@
       </c>
     </row>
     <row r="86" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B86" s="67"/>
+      <c r="B86" s="66"/>
       <c r="C86" s="4">
         <v>0.86805555555555547</v>
       </c>
@@ -3792,7 +3792,7 @@
       </c>
     </row>
     <row r="87" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B87" s="67" t="s">
+      <c r="B87" s="66" t="s">
         <v>43</v>
       </c>
       <c r="C87" s="4">
@@ -3823,7 +3823,7 @@
       </c>
     </row>
     <row r="88" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B88" s="67"/>
+      <c r="B88" s="66"/>
       <c r="C88" s="4">
         <v>0.88541666666666663</v>
       </c>
@@ -3883,7 +3883,7 @@
       </c>
     </row>
     <row r="90" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B90" s="67" t="s">
+      <c r="B90" s="66" t="s">
         <v>45</v>
       </c>
       <c r="C90" s="4">
@@ -3914,7 +3914,7 @@
       </c>
     </row>
     <row r="91" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B91" s="67"/>
+      <c r="B91" s="66"/>
       <c r="C91" s="4">
         <v>0.3576388888888889</v>
       </c>
@@ -3943,7 +3943,7 @@
       </c>
     </row>
     <row r="92" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B92" s="67"/>
+      <c r="B92" s="66"/>
       <c r="C92" s="4">
         <v>0.39583333333333331</v>
       </c>
@@ -3972,7 +3972,7 @@
       </c>
     </row>
     <row r="93" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B93" s="67"/>
+      <c r="B93" s="66"/>
       <c r="C93" s="4">
         <v>0.4548611111111111</v>
       </c>
@@ -4001,7 +4001,7 @@
       </c>
     </row>
     <row r="94" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B94" s="67"/>
+      <c r="B94" s="66"/>
       <c r="C94" s="4">
         <v>0.48958333333333331</v>
       </c>
@@ -4030,7 +4030,7 @@
       </c>
     </row>
     <row r="95" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B95" s="67" t="s">
+      <c r="B95" s="66" t="s">
         <v>46</v>
       </c>
       <c r="C95" s="4">
@@ -4061,7 +4061,7 @@
       </c>
     </row>
     <row r="96" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B96" s="67"/>
+      <c r="B96" s="66"/>
       <c r="C96" s="4">
         <v>0.5</v>
       </c>
@@ -4090,7 +4090,7 @@
       </c>
     </row>
     <row r="97" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B97" s="67"/>
+      <c r="B97" s="66"/>
       <c r="C97" s="4">
         <v>0.70138888888888884</v>
       </c>
@@ -4119,7 +4119,7 @@
       </c>
     </row>
     <row r="98" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B98" s="67" t="s">
+      <c r="B98" s="66" t="s">
         <v>47</v>
       </c>
       <c r="C98" s="4">
@@ -4150,7 +4150,7 @@
       </c>
     </row>
     <row r="99" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B99" s="67"/>
+      <c r="B99" s="66"/>
       <c r="C99" s="4">
         <v>0.51736111111111105</v>
       </c>
@@ -4179,7 +4179,7 @@
       </c>
     </row>
     <row r="100" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B100" s="67"/>
+      <c r="B100" s="66"/>
       <c r="C100" s="4">
         <v>0.67361111111111116</v>
       </c>
@@ -4208,7 +4208,7 @@
       </c>
     </row>
     <row r="101" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B101" s="67" t="s">
+      <c r="B101" s="66" t="s">
         <v>48</v>
       </c>
       <c r="C101" s="4">
@@ -4239,7 +4239,7 @@
       </c>
     </row>
     <row r="102" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B102" s="67"/>
+      <c r="B102" s="66"/>
       <c r="C102" s="4">
         <v>0.65277777777777779</v>
       </c>
@@ -4268,7 +4268,7 @@
       </c>
     </row>
     <row r="103" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B103" s="67" t="s">
+      <c r="B103" s="66" t="s">
         <v>50</v>
       </c>
       <c r="C103" s="4">
@@ -4302,7 +4302,7 @@
       </c>
     </row>
     <row r="104" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B104" s="67"/>
+      <c r="B104" s="66"/>
       <c r="C104" s="4">
         <v>0.56944444444444442</v>
       </c>
@@ -4331,7 +4331,7 @@
       </c>
     </row>
     <row r="105" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B105" s="67"/>
+      <c r="B105" s="66"/>
       <c r="C105" s="4">
         <v>0.68055555555555547</v>
       </c>
@@ -4363,7 +4363,7 @@
       </c>
     </row>
     <row r="106" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B106" s="67"/>
+      <c r="B106" s="66"/>
       <c r="C106" s="4">
         <v>0.70486111111111116</v>
       </c>
@@ -4392,7 +4392,7 @@
       </c>
     </row>
     <row r="107" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B107" s="67" t="s">
+      <c r="B107" s="66" t="s">
         <v>51</v>
       </c>
       <c r="C107" s="4">
@@ -4423,7 +4423,7 @@
       </c>
     </row>
     <row r="108" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B108" s="67"/>
+      <c r="B108" s="66"/>
       <c r="C108" s="4">
         <v>0.98958333333333337</v>
       </c>
@@ -4452,7 +4452,7 @@
       </c>
     </row>
     <row r="109" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B109" s="67" t="s">
+      <c r="B109" s="66" t="s">
         <v>52</v>
       </c>
       <c r="C109" s="4">
@@ -4483,7 +4483,7 @@
       </c>
     </row>
     <row r="110" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B110" s="67"/>
+      <c r="B110" s="66"/>
       <c r="C110" s="4">
         <v>0.61458333333333337</v>
       </c>
@@ -4512,7 +4512,7 @@
       </c>
     </row>
     <row r="111" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B111" s="67"/>
+      <c r="B111" s="66"/>
       <c r="C111" s="4">
         <v>0.66319444444444442</v>
       </c>
@@ -4541,7 +4541,7 @@
       </c>
     </row>
     <row r="112" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B112" s="67"/>
+      <c r="B112" s="66"/>
       <c r="C112" s="4">
         <v>0.73958333333333337</v>
       </c>
@@ -4570,7 +4570,7 @@
       </c>
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B113" s="67"/>
+      <c r="B113" s="66"/>
       <c r="C113" s="4">
         <v>0.80555555555555547</v>
       </c>
@@ -4599,7 +4599,7 @@
       </c>
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B114" s="67" t="s">
+      <c r="B114" s="66" t="s">
         <v>53</v>
       </c>
       <c r="C114" s="4">
@@ -4630,7 +4630,7 @@
       </c>
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B115" s="67"/>
+      <c r="B115" s="66"/>
       <c r="C115" s="4">
         <v>0.69097222222222221</v>
       </c>
@@ -4693,7 +4693,7 @@
       </c>
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B117" s="67" t="s">
+      <c r="B117" s="66" t="s">
         <v>55</v>
       </c>
       <c r="C117" s="4">
@@ -4724,7 +4724,7 @@
       </c>
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B118" s="67"/>
+      <c r="B118" s="66"/>
       <c r="C118" s="4">
         <v>0.51736111111111105</v>
       </c>
@@ -4753,7 +4753,7 @@
       </c>
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B119" s="67"/>
+      <c r="B119" s="66"/>
       <c r="C119" s="4">
         <v>0.59375</v>
       </c>
@@ -4782,7 +4782,7 @@
       </c>
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B120" s="67"/>
+      <c r="B120" s="66"/>
       <c r="C120" s="4">
         <v>0.65277777777777779</v>
       </c>
@@ -4811,7 +4811,7 @@
       </c>
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B121" s="70"/>
+      <c r="B121" s="69"/>
       <c r="C121" s="38">
         <v>0.77777777777777779</v>
       </c>
@@ -4860,10 +4860,10 @@
       <c r="B123" s="51"/>
       <c r="C123" s="11"/>
       <c r="D123" s="11"/>
-      <c r="E123" s="68" t="s">
+      <c r="E123" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="F123" s="69" t="s">
+      <c r="F123" s="68" t="s">
         <v>18</v>
       </c>
       <c r="G123" s="17" t="s">
@@ -4886,8 +4886,8 @@
       <c r="D124" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E124" s="68"/>
-      <c r="F124" s="69"/>
+      <c r="E124" s="67"/>
+      <c r="F124" s="68"/>
       <c r="G124" s="12" t="s">
         <v>14</v>
       </c>
@@ -8700,27 +8700,34 @@
       <c r="B255" s="49" t="s">
         <v>97</v>
       </c>
-      <c r="C255" s="4"/>
-      <c r="D255" s="18"/>
+      <c r="C255" s="4">
+        <v>0.61736111111111114</v>
+      </c>
+      <c r="D255" s="18">
+        <v>0.6381944444444444</v>
+      </c>
       <c r="E255" s="20">
         <f t="shared" si="66"/>
-        <v>0</v>
+        <v>2.0833333333333259E-2</v>
       </c>
       <c r="F255" s="21">
         <f t="shared" si="67"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G255" s="15">
         <f t="shared" si="68"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H255" s="15">
         <f t="shared" si="69"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555568</v>
       </c>
       <c r="I255" s="23">
         <f t="shared" si="70"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
+      </c>
+      <c r="J255" s="1" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="256" spans="2:10" x14ac:dyDescent="0.25">
@@ -8732,19 +8739,19 @@
       </c>
       <c r="F256" s="21">
         <f t="shared" si="67"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G256" s="15">
         <f t="shared" si="68"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H256" s="15">
         <f t="shared" si="69"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I256" s="23">
         <f t="shared" si="70"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="257" spans="3:9" x14ac:dyDescent="0.25">
@@ -8756,19 +8763,19 @@
       </c>
       <c r="F257" s="21">
         <f t="shared" si="67"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G257" s="15">
         <f t="shared" si="68"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H257" s="15">
         <f t="shared" si="69"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I257" s="23">
         <f t="shared" si="70"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="258" spans="3:9" x14ac:dyDescent="0.25">
@@ -8780,19 +8787,19 @@
       </c>
       <c r="F258" s="21">
         <f t="shared" si="67"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G258" s="15">
         <f t="shared" si="68"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H258" s="15">
         <f t="shared" si="69"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I258" s="23">
         <f t="shared" si="70"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="259" spans="3:9" x14ac:dyDescent="0.25">
@@ -8804,19 +8811,19 @@
       </c>
       <c r="F259" s="21">
         <f t="shared" si="67"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G259" s="15">
         <f t="shared" si="68"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H259" s="15">
         <f t="shared" si="69"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I259" s="23">
         <f t="shared" si="70"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="260" spans="3:9" x14ac:dyDescent="0.25">
@@ -8828,19 +8835,19 @@
       </c>
       <c r="F260" s="21">
         <f t="shared" si="67"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G260" s="15">
         <f t="shared" si="68"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H260" s="15">
         <f t="shared" si="69"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I260" s="23">
         <f t="shared" si="70"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="261" spans="3:9" x14ac:dyDescent="0.25">
@@ -8852,19 +8859,19 @@
       </c>
       <c r="F261" s="21">
         <f t="shared" si="67"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G261" s="15">
         <f t="shared" si="68"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H261" s="15">
         <f t="shared" si="69"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I261" s="23">
         <f t="shared" si="70"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="262" spans="3:9" x14ac:dyDescent="0.25">
@@ -8876,19 +8883,19 @@
       </c>
       <c r="F262" s="21">
         <f t="shared" si="67"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G262" s="15">
         <f t="shared" si="68"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H262" s="15">
         <f t="shared" si="69"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I262" s="23">
         <f t="shared" si="70"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="263" spans="3:9" x14ac:dyDescent="0.25">
@@ -8900,19 +8907,19 @@
       </c>
       <c r="F263" s="21">
         <f t="shared" si="67"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G263" s="15">
         <f t="shared" si="68"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H263" s="15">
         <f t="shared" si="69"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I263" s="23">
         <f t="shared" si="70"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="264" spans="3:9" x14ac:dyDescent="0.25">
@@ -8924,19 +8931,19 @@
       </c>
       <c r="F264" s="21">
         <f t="shared" si="67"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G264" s="15">
         <f t="shared" si="68"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H264" s="15">
         <f t="shared" si="69"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I264" s="23">
         <f t="shared" si="70"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="265" spans="3:9" x14ac:dyDescent="0.25">
@@ -8948,19 +8955,19 @@
       </c>
       <c r="F265" s="21">
         <f t="shared" si="67"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G265" s="15">
         <f t="shared" si="68"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H265" s="15">
         <f t="shared" si="69"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I265" s="23">
         <f t="shared" si="70"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="266" spans="3:9" x14ac:dyDescent="0.25">
@@ -8972,19 +8979,19 @@
       </c>
       <c r="F266" s="21">
         <f t="shared" si="67"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G266" s="15">
         <f t="shared" si="68"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H266" s="15">
         <f t="shared" si="69"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I266" s="23">
         <f t="shared" si="70"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="267" spans="3:9" x14ac:dyDescent="0.25">
@@ -8996,19 +9003,19 @@
       </c>
       <c r="F267" s="21">
         <f t="shared" si="67"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G267" s="15">
         <f t="shared" si="68"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H267" s="15">
         <f t="shared" si="69"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I267" s="23">
         <f t="shared" si="70"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="268" spans="3:9" x14ac:dyDescent="0.25">
@@ -9020,19 +9027,19 @@
       </c>
       <c r="F268" s="21">
         <f t="shared" si="67"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G268" s="15">
         <f t="shared" si="68"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H268" s="15">
         <f t="shared" si="69"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I268" s="23">
         <f t="shared" si="70"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="269" spans="3:9" x14ac:dyDescent="0.25">
@@ -9044,19 +9051,19 @@
       </c>
       <c r="F269" s="21">
         <f t="shared" si="67"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G269" s="15">
         <f t="shared" si="68"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H269" s="15">
         <f t="shared" si="69"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I269" s="23">
         <f t="shared" si="70"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="270" spans="3:9" x14ac:dyDescent="0.25">
@@ -9068,19 +9075,19 @@
       </c>
       <c r="F270" s="21">
         <f t="shared" si="67"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G270" s="15">
         <f t="shared" si="68"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H270" s="15">
         <f t="shared" si="69"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I270" s="23">
         <f t="shared" si="70"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="271" spans="3:9" x14ac:dyDescent="0.25">
@@ -9092,19 +9099,19 @@
       </c>
       <c r="F271" s="21">
         <f t="shared" si="67"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G271" s="15">
         <f t="shared" si="68"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H271" s="15">
         <f t="shared" si="69"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I271" s="23">
         <f t="shared" si="70"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="272" spans="3:9" x14ac:dyDescent="0.25">
@@ -9116,19 +9123,19 @@
       </c>
       <c r="F272" s="21">
         <f t="shared" si="67"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G272" s="15">
         <f t="shared" si="68"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H272" s="15">
         <f t="shared" si="69"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I272" s="23">
         <f t="shared" si="70"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="273" spans="3:9" x14ac:dyDescent="0.25">
@@ -9140,19 +9147,19 @@
       </c>
       <c r="F273" s="21">
         <f t="shared" si="67"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G273" s="15">
         <f t="shared" si="68"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H273" s="15">
         <f t="shared" si="69"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I273" s="23">
         <f t="shared" si="70"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="274" spans="3:9" x14ac:dyDescent="0.25">
@@ -9164,19 +9171,19 @@
       </c>
       <c r="F274" s="21">
         <f t="shared" si="67"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G274" s="15">
         <f t="shared" si="68"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H274" s="15">
         <f t="shared" si="69"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I274" s="23">
         <f t="shared" si="70"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="275" spans="3:9" x14ac:dyDescent="0.25">
@@ -9188,19 +9195,19 @@
       </c>
       <c r="F275" s="21">
         <f t="shared" si="67"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G275" s="15">
         <f t="shared" si="68"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H275" s="15">
         <f t="shared" si="69"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I275" s="23">
         <f t="shared" si="70"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="276" spans="3:9" x14ac:dyDescent="0.25">
@@ -9212,19 +9219,19 @@
       </c>
       <c r="F276" s="21">
         <f t="shared" si="67"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G276" s="15">
         <f t="shared" si="68"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H276" s="15">
         <f t="shared" si="69"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I276" s="23">
         <f t="shared" si="70"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="277" spans="3:9" x14ac:dyDescent="0.25">
@@ -9236,19 +9243,19 @@
       </c>
       <c r="F277" s="21">
         <f t="shared" si="67"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G277" s="15">
         <f t="shared" si="68"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H277" s="15">
         <f t="shared" si="69"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I277" s="23">
         <f t="shared" si="70"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="278" spans="3:9" x14ac:dyDescent="0.25">
@@ -9260,19 +9267,19 @@
       </c>
       <c r="F278" s="21">
         <f t="shared" si="67"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G278" s="15">
         <f t="shared" si="68"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H278" s="15">
         <f t="shared" si="69"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I278" s="23">
         <f t="shared" si="70"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="279" spans="3:9" x14ac:dyDescent="0.25">
@@ -9284,19 +9291,19 @@
       </c>
       <c r="F279" s="21">
         <f t="shared" si="67"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G279" s="15">
         <f t="shared" si="68"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H279" s="15">
         <f t="shared" si="69"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I279" s="23">
         <f t="shared" si="70"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="280" spans="3:9" x14ac:dyDescent="0.25">
@@ -9308,19 +9315,19 @@
       </c>
       <c r="F280" s="21">
         <f t="shared" si="67"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G280" s="15">
         <f t="shared" si="68"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H280" s="15">
         <f t="shared" si="69"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I280" s="23">
         <f t="shared" si="70"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="281" spans="3:9" x14ac:dyDescent="0.25">
@@ -9332,19 +9339,19 @@
       </c>
       <c r="F281" s="21">
         <f t="shared" si="67"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G281" s="15">
         <f t="shared" si="68"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H281" s="15">
         <f t="shared" si="69"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I281" s="23">
         <f t="shared" si="70"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="282" spans="3:9" x14ac:dyDescent="0.25">
@@ -9356,19 +9363,19 @@
       </c>
       <c r="F282" s="21">
         <f t="shared" ref="F282:F342" si="72">F281+E282</f>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G282" s="15">
         <f t="shared" ref="G282:G342" si="73">F282</f>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H282" s="15">
         <f t="shared" ref="H282:H342" si="74">(H281+G282-G281)</f>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I282" s="23">
         <f t="shared" ref="I282:I342" si="75">H282*24*$J$32</f>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="283" spans="3:9" x14ac:dyDescent="0.25">
@@ -9380,19 +9387,19 @@
       </c>
       <c r="F283" s="21">
         <f t="shared" si="72"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G283" s="15">
         <f t="shared" si="73"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H283" s="15">
         <f t="shared" si="74"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I283" s="23">
         <f t="shared" si="75"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="284" spans="3:9" x14ac:dyDescent="0.25">
@@ -9404,19 +9411,19 @@
       </c>
       <c r="F284" s="21">
         <f t="shared" si="72"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G284" s="15">
         <f t="shared" si="73"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H284" s="15">
         <f t="shared" si="74"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I284" s="23">
         <f t="shared" si="75"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="285" spans="3:9" x14ac:dyDescent="0.25">
@@ -9428,19 +9435,19 @@
       </c>
       <c r="F285" s="21">
         <f t="shared" si="72"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G285" s="15">
         <f t="shared" si="73"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H285" s="15">
         <f t="shared" si="74"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I285" s="23">
         <f t="shared" si="75"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="286" spans="3:9" x14ac:dyDescent="0.25">
@@ -9452,19 +9459,19 @@
       </c>
       <c r="F286" s="21">
         <f t="shared" si="72"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G286" s="15">
         <f t="shared" si="73"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H286" s="15">
         <f t="shared" si="74"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I286" s="23">
         <f t="shared" si="75"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="287" spans="3:9" x14ac:dyDescent="0.25">
@@ -9476,19 +9483,19 @@
       </c>
       <c r="F287" s="21">
         <f t="shared" si="72"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G287" s="15">
         <f t="shared" si="73"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H287" s="15">
         <f t="shared" si="74"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I287" s="23">
         <f t="shared" si="75"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="288" spans="3:9" x14ac:dyDescent="0.25">
@@ -9500,19 +9507,19 @@
       </c>
       <c r="F288" s="21">
         <f t="shared" si="72"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G288" s="15">
         <f t="shared" si="73"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H288" s="15">
         <f t="shared" si="74"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I288" s="23">
         <f t="shared" si="75"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="289" spans="3:9" x14ac:dyDescent="0.25">
@@ -9524,19 +9531,19 @@
       </c>
       <c r="F289" s="21">
         <f t="shared" si="72"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G289" s="15">
         <f t="shared" si="73"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H289" s="15">
         <f t="shared" si="74"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I289" s="23">
         <f t="shared" si="75"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="290" spans="3:9" x14ac:dyDescent="0.25">
@@ -9548,19 +9555,19 @@
       </c>
       <c r="F290" s="21">
         <f t="shared" si="72"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G290" s="15">
         <f t="shared" si="73"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H290" s="15">
         <f t="shared" si="74"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I290" s="23">
         <f t="shared" si="75"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="291" spans="3:9" x14ac:dyDescent="0.25">
@@ -9572,19 +9579,19 @@
       </c>
       <c r="F291" s="21">
         <f t="shared" si="72"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G291" s="15">
         <f t="shared" si="73"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H291" s="15">
         <f t="shared" si="74"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I291" s="23">
         <f t="shared" si="75"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="292" spans="3:9" x14ac:dyDescent="0.25">
@@ -9596,19 +9603,19 @@
       </c>
       <c r="F292" s="21">
         <f t="shared" si="72"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G292" s="15">
         <f t="shared" si="73"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H292" s="15">
         <f t="shared" si="74"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I292" s="23">
         <f t="shared" si="75"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="293" spans="3:9" x14ac:dyDescent="0.25">
@@ -9620,19 +9627,19 @@
       </c>
       <c r="F293" s="21">
         <f t="shared" si="72"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G293" s="15">
         <f t="shared" si="73"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H293" s="15">
         <f t="shared" si="74"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I293" s="23">
         <f t="shared" si="75"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="294" spans="3:9" x14ac:dyDescent="0.25">
@@ -9644,19 +9651,19 @@
       </c>
       <c r="F294" s="21">
         <f t="shared" si="72"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G294" s="15">
         <f t="shared" si="73"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H294" s="15">
         <f t="shared" si="74"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I294" s="23">
         <f t="shared" si="75"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="295" spans="3:9" x14ac:dyDescent="0.25">
@@ -9668,19 +9675,19 @@
       </c>
       <c r="F295" s="21">
         <f t="shared" si="72"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G295" s="15">
         <f t="shared" si="73"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H295" s="15">
         <f t="shared" si="74"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I295" s="23">
         <f t="shared" si="75"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="296" spans="3:9" x14ac:dyDescent="0.25">
@@ -9692,19 +9699,19 @@
       </c>
       <c r="F296" s="21">
         <f t="shared" si="72"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G296" s="15">
         <f t="shared" si="73"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H296" s="15">
         <f t="shared" si="74"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I296" s="23">
         <f t="shared" si="75"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="297" spans="3:9" x14ac:dyDescent="0.25">
@@ -9716,19 +9723,19 @@
       </c>
       <c r="F297" s="21">
         <f t="shared" si="72"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G297" s="15">
         <f t="shared" si="73"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H297" s="15">
         <f t="shared" si="74"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I297" s="23">
         <f t="shared" si="75"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="298" spans="3:9" x14ac:dyDescent="0.25">
@@ -9740,19 +9747,19 @@
       </c>
       <c r="F298" s="21">
         <f t="shared" si="72"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G298" s="15">
         <f t="shared" si="73"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H298" s="15">
         <f t="shared" si="74"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I298" s="23">
         <f t="shared" si="75"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="299" spans="3:9" x14ac:dyDescent="0.25">
@@ -9764,19 +9771,19 @@
       </c>
       <c r="F299" s="21">
         <f t="shared" si="72"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G299" s="15">
         <f t="shared" si="73"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H299" s="15">
         <f t="shared" si="74"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I299" s="23">
         <f t="shared" si="75"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="300" spans="3:9" x14ac:dyDescent="0.25">
@@ -9788,19 +9795,19 @@
       </c>
       <c r="F300" s="21">
         <f t="shared" si="72"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G300" s="15">
         <f t="shared" si="73"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H300" s="15">
         <f t="shared" si="74"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I300" s="23">
         <f t="shared" si="75"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="301" spans="3:9" x14ac:dyDescent="0.25">
@@ -9812,19 +9819,19 @@
       </c>
       <c r="F301" s="21">
         <f t="shared" si="72"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G301" s="15">
         <f t="shared" si="73"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H301" s="15">
         <f t="shared" si="74"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I301" s="23">
         <f t="shared" si="75"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="302" spans="3:9" x14ac:dyDescent="0.25">
@@ -9836,19 +9843,19 @@
       </c>
       <c r="F302" s="21">
         <f t="shared" si="72"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G302" s="15">
         <f t="shared" si="73"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H302" s="15">
         <f t="shared" si="74"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I302" s="23">
         <f t="shared" si="75"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="303" spans="3:9" x14ac:dyDescent="0.25">
@@ -9860,19 +9867,19 @@
       </c>
       <c r="F303" s="21">
         <f t="shared" si="72"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G303" s="15">
         <f t="shared" si="73"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H303" s="15">
         <f t="shared" si="74"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I303" s="23">
         <f t="shared" si="75"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="304" spans="3:9" x14ac:dyDescent="0.25">
@@ -9884,19 +9891,19 @@
       </c>
       <c r="F304" s="21">
         <f t="shared" si="72"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G304" s="15">
         <f t="shared" si="73"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H304" s="15">
         <f t="shared" si="74"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I304" s="23">
         <f t="shared" si="75"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="305" spans="3:9" x14ac:dyDescent="0.25">
@@ -9908,19 +9915,19 @@
       </c>
       <c r="F305" s="21">
         <f t="shared" si="72"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G305" s="15">
         <f t="shared" si="73"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H305" s="15">
         <f t="shared" si="74"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I305" s="23">
         <f t="shared" si="75"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="306" spans="3:9" x14ac:dyDescent="0.25">
@@ -9932,19 +9939,19 @@
       </c>
       <c r="F306" s="21">
         <f t="shared" si="72"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G306" s="15">
         <f t="shared" si="73"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H306" s="15">
         <f t="shared" si="74"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I306" s="23">
         <f t="shared" si="75"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="307" spans="3:9" x14ac:dyDescent="0.25">
@@ -9956,19 +9963,19 @@
       </c>
       <c r="F307" s="21">
         <f t="shared" si="72"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G307" s="15">
         <f t="shared" si="73"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H307" s="15">
         <f t="shared" si="74"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I307" s="23">
         <f t="shared" si="75"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="308" spans="3:9" x14ac:dyDescent="0.25">
@@ -9980,19 +9987,19 @@
       </c>
       <c r="F308" s="21">
         <f t="shared" si="72"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G308" s="15">
         <f t="shared" si="73"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H308" s="15">
         <f t="shared" si="74"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I308" s="23">
         <f t="shared" si="75"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="309" spans="3:9" x14ac:dyDescent="0.25">
@@ -10004,19 +10011,19 @@
       </c>
       <c r="F309" s="21">
         <f t="shared" si="72"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G309" s="15">
         <f t="shared" si="73"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H309" s="15">
         <f t="shared" si="74"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I309" s="23">
         <f t="shared" si="75"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="310" spans="3:9" x14ac:dyDescent="0.25">
@@ -10028,19 +10035,19 @@
       </c>
       <c r="F310" s="21">
         <f t="shared" si="72"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G310" s="15">
         <f t="shared" si="73"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H310" s="15">
         <f t="shared" si="74"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I310" s="23">
         <f t="shared" si="75"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="311" spans="3:9" x14ac:dyDescent="0.25">
@@ -10052,19 +10059,19 @@
       </c>
       <c r="F311" s="21">
         <f t="shared" si="72"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G311" s="15">
         <f t="shared" si="73"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H311" s="15">
         <f t="shared" si="74"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I311" s="23">
         <f t="shared" si="75"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="312" spans="3:9" x14ac:dyDescent="0.25">
@@ -10076,19 +10083,19 @@
       </c>
       <c r="F312" s="21">
         <f t="shared" si="72"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G312" s="15">
         <f t="shared" si="73"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H312" s="15">
         <f t="shared" si="74"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I312" s="23">
         <f t="shared" si="75"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="313" spans="3:9" x14ac:dyDescent="0.25">
@@ -10100,19 +10107,19 @@
       </c>
       <c r="F313" s="21">
         <f t="shared" si="72"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G313" s="15">
         <f t="shared" si="73"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H313" s="15">
         <f t="shared" si="74"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I313" s="23">
         <f t="shared" si="75"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="314" spans="3:9" x14ac:dyDescent="0.25">
@@ -10124,19 +10131,19 @@
       </c>
       <c r="F314" s="21">
         <f t="shared" si="72"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G314" s="15">
         <f t="shared" si="73"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H314" s="15">
         <f t="shared" si="74"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I314" s="23">
         <f t="shared" si="75"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="315" spans="3:9" x14ac:dyDescent="0.25">
@@ -10148,19 +10155,19 @@
       </c>
       <c r="F315" s="21">
         <f t="shared" si="72"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G315" s="15">
         <f t="shared" si="73"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H315" s="15">
         <f t="shared" si="74"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I315" s="23">
         <f t="shared" si="75"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="316" spans="3:9" x14ac:dyDescent="0.25">
@@ -10172,19 +10179,19 @@
       </c>
       <c r="F316" s="21">
         <f t="shared" si="72"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G316" s="15">
         <f t="shared" si="73"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H316" s="15">
         <f t="shared" si="74"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I316" s="23">
         <f t="shared" si="75"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="317" spans="3:9" x14ac:dyDescent="0.25">
@@ -10196,19 +10203,19 @@
       </c>
       <c r="F317" s="21">
         <f t="shared" si="72"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G317" s="15">
         <f t="shared" si="73"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H317" s="15">
         <f t="shared" si="74"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I317" s="23">
         <f t="shared" si="75"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="318" spans="3:9" x14ac:dyDescent="0.25">
@@ -10220,19 +10227,19 @@
       </c>
       <c r="F318" s="21">
         <f t="shared" si="72"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G318" s="15">
         <f t="shared" si="73"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H318" s="15">
         <f t="shared" si="74"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I318" s="23">
         <f t="shared" si="75"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="319" spans="3:9" x14ac:dyDescent="0.25">
@@ -10244,19 +10251,19 @@
       </c>
       <c r="F319" s="21">
         <f t="shared" si="72"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G319" s="15">
         <f t="shared" si="73"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H319" s="15">
         <f t="shared" si="74"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I319" s="23">
         <f t="shared" si="75"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="320" spans="3:9" x14ac:dyDescent="0.25">
@@ -10268,19 +10275,19 @@
       </c>
       <c r="F320" s="21">
         <f t="shared" si="72"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G320" s="15">
         <f t="shared" si="73"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H320" s="15">
         <f t="shared" si="74"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I320" s="23">
         <f t="shared" si="75"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="321" spans="3:9" x14ac:dyDescent="0.25">
@@ -10292,19 +10299,19 @@
       </c>
       <c r="F321" s="21">
         <f t="shared" si="72"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G321" s="15">
         <f t="shared" si="73"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H321" s="15">
         <f t="shared" si="74"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I321" s="23">
         <f t="shared" si="75"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="322" spans="3:9" x14ac:dyDescent="0.25">
@@ -10316,19 +10323,19 @@
       </c>
       <c r="F322" s="21">
         <f t="shared" si="72"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G322" s="15">
         <f t="shared" si="73"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H322" s="15">
         <f t="shared" si="74"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I322" s="23">
         <f t="shared" si="75"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="323" spans="3:9" x14ac:dyDescent="0.25">
@@ -10340,19 +10347,19 @@
       </c>
       <c r="F323" s="21">
         <f t="shared" si="72"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G323" s="15">
         <f t="shared" si="73"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H323" s="15">
         <f t="shared" si="74"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I323" s="23">
         <f t="shared" si="75"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="324" spans="3:9" x14ac:dyDescent="0.25">
@@ -10364,19 +10371,19 @@
       </c>
       <c r="F324" s="21">
         <f t="shared" si="72"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G324" s="15">
         <f t="shared" si="73"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H324" s="15">
         <f t="shared" si="74"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I324" s="23">
         <f t="shared" si="75"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="325" spans="3:9" x14ac:dyDescent="0.25">
@@ -10388,19 +10395,19 @@
       </c>
       <c r="F325" s="21">
         <f t="shared" si="72"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G325" s="15">
         <f t="shared" si="73"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H325" s="15">
         <f t="shared" si="74"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I325" s="23">
         <f t="shared" si="75"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="326" spans="3:9" x14ac:dyDescent="0.25">
@@ -10412,19 +10419,19 @@
       </c>
       <c r="F326" s="21">
         <f t="shared" si="72"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G326" s="15">
         <f t="shared" si="73"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H326" s="15">
         <f t="shared" si="74"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I326" s="23">
         <f t="shared" si="75"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="327" spans="3:9" x14ac:dyDescent="0.25">
@@ -10436,19 +10443,19 @@
       </c>
       <c r="F327" s="21">
         <f t="shared" si="72"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G327" s="15">
         <f t="shared" si="73"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H327" s="15">
         <f t="shared" si="74"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I327" s="23">
         <f t="shared" si="75"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="328" spans="3:9" x14ac:dyDescent="0.25">
@@ -10460,19 +10467,19 @@
       </c>
       <c r="F328" s="21">
         <f t="shared" si="72"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G328" s="15">
         <f t="shared" si="73"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H328" s="15">
         <f t="shared" si="74"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I328" s="23">
         <f t="shared" si="75"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="329" spans="3:9" x14ac:dyDescent="0.25">
@@ -10484,19 +10491,19 @@
       </c>
       <c r="F329" s="21">
         <f t="shared" si="72"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G329" s="15">
         <f t="shared" si="73"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H329" s="15">
         <f t="shared" si="74"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I329" s="23">
         <f t="shared" si="75"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="330" spans="3:9" x14ac:dyDescent="0.25">
@@ -10508,19 +10515,19 @@
       </c>
       <c r="F330" s="21">
         <f t="shared" si="72"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G330" s="15">
         <f t="shared" si="73"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H330" s="15">
         <f t="shared" si="74"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I330" s="23">
         <f t="shared" si="75"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="331" spans="3:9" x14ac:dyDescent="0.25">
@@ -10532,19 +10539,19 @@
       </c>
       <c r="F331" s="21">
         <f t="shared" si="72"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G331" s="15">
         <f t="shared" si="73"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H331" s="15">
         <f t="shared" si="74"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I331" s="23">
         <f t="shared" si="75"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="332" spans="3:9" x14ac:dyDescent="0.25">
@@ -10556,19 +10563,19 @@
       </c>
       <c r="F332" s="21">
         <f t="shared" si="72"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G332" s="15">
         <f t="shared" si="73"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H332" s="15">
         <f t="shared" si="74"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I332" s="23">
         <f t="shared" si="75"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="333" spans="3:9" x14ac:dyDescent="0.25">
@@ -10580,19 +10587,19 @@
       </c>
       <c r="F333" s="21">
         <f t="shared" si="72"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G333" s="15">
         <f t="shared" si="73"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H333" s="15">
         <f t="shared" si="74"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I333" s="23">
         <f t="shared" si="75"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="334" spans="3:9" x14ac:dyDescent="0.25">
@@ -10604,19 +10611,19 @@
       </c>
       <c r="F334" s="21">
         <f t="shared" si="72"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G334" s="15">
         <f t="shared" si="73"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H334" s="15">
         <f t="shared" si="74"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I334" s="23">
         <f t="shared" si="75"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="335" spans="3:9" x14ac:dyDescent="0.25">
@@ -10628,19 +10635,19 @@
       </c>
       <c r="F335" s="21">
         <f t="shared" si="72"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G335" s="15">
         <f t="shared" si="73"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H335" s="15">
         <f t="shared" si="74"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I335" s="23">
         <f t="shared" si="75"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="336" spans="3:9" x14ac:dyDescent="0.25">
@@ -10652,19 +10659,19 @@
       </c>
       <c r="F336" s="21">
         <f t="shared" si="72"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G336" s="15">
         <f t="shared" si="73"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H336" s="15">
         <f t="shared" si="74"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I336" s="23">
         <f t="shared" si="75"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="337" spans="3:9" x14ac:dyDescent="0.25">
@@ -10676,19 +10683,19 @@
       </c>
       <c r="F337" s="21">
         <f t="shared" si="72"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G337" s="15">
         <f t="shared" si="73"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H337" s="15">
         <f t="shared" si="74"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I337" s="23">
         <f t="shared" si="75"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="338" spans="3:9" x14ac:dyDescent="0.25">
@@ -10700,19 +10707,19 @@
       </c>
       <c r="F338" s="21">
         <f t="shared" si="72"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G338" s="15">
         <f t="shared" si="73"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H338" s="15">
         <f t="shared" si="74"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I338" s="23">
         <f t="shared" si="75"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="339" spans="3:9" x14ac:dyDescent="0.25">
@@ -10724,19 +10731,19 @@
       </c>
       <c r="F339" s="21">
         <f t="shared" si="72"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G339" s="15">
         <f t="shared" si="73"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H339" s="15">
         <f t="shared" si="74"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I339" s="23">
         <f t="shared" si="75"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="340" spans="3:9" x14ac:dyDescent="0.25">
@@ -10748,19 +10755,19 @@
       </c>
       <c r="F340" s="21">
         <f t="shared" si="72"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G340" s="15">
         <f t="shared" si="73"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H340" s="15">
         <f t="shared" si="74"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I340" s="23">
         <f t="shared" si="75"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="341" spans="3:9" x14ac:dyDescent="0.25">
@@ -10772,19 +10779,19 @@
       </c>
       <c r="F341" s="21">
         <f t="shared" si="72"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G341" s="15">
         <f t="shared" si="73"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H341" s="15">
         <f t="shared" si="74"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I341" s="23">
         <f t="shared" si="75"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
     <row r="342" spans="3:9" x14ac:dyDescent="0.25">
@@ -10796,23 +10803,68 @@
       </c>
       <c r="F342" s="21">
         <f t="shared" si="72"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="G342" s="15">
         <f t="shared" si="73"/>
-        <v>3.7909722222222211</v>
+        <v>3.8118055555555541</v>
       </c>
       <c r="H342" s="15">
         <f t="shared" si="74"/>
-        <v>5.8534722222222246</v>
+        <v>5.8743055555555559</v>
       </c>
       <c r="I342" s="23">
         <f t="shared" si="75"/>
-        <v>23882.166666666679</v>
+        <v>23967.166666666668</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="61">
+    <mergeCell ref="B240:B245"/>
+    <mergeCell ref="B237:B239"/>
+    <mergeCell ref="B230:B236"/>
+    <mergeCell ref="B210:B212"/>
+    <mergeCell ref="B204:B209"/>
+    <mergeCell ref="B213:B219"/>
+    <mergeCell ref="B201:B203"/>
+    <mergeCell ref="B228:B229"/>
+    <mergeCell ref="B220:B227"/>
+    <mergeCell ref="B195:B200"/>
+    <mergeCell ref="B172:B174"/>
+    <mergeCell ref="B175:B177"/>
+    <mergeCell ref="B178:B183"/>
+    <mergeCell ref="B184:B187"/>
+    <mergeCell ref="B188:B192"/>
+    <mergeCell ref="B164:B170"/>
+    <mergeCell ref="B151:B155"/>
+    <mergeCell ref="B156:B162"/>
+    <mergeCell ref="B142:B144"/>
+    <mergeCell ref="K13:K17"/>
+    <mergeCell ref="K18:K22"/>
+    <mergeCell ref="B14:B18"/>
+    <mergeCell ref="B19:B23"/>
+    <mergeCell ref="B47:B53"/>
+    <mergeCell ref="B41:B46"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="B33:B35"/>
+    <mergeCell ref="B37:B40"/>
+    <mergeCell ref="B73:B74"/>
+    <mergeCell ref="B70:B71"/>
+    <mergeCell ref="E123:E124"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="B24:B27"/>
+    <mergeCell ref="B66:B69"/>
+    <mergeCell ref="B63:B65"/>
+    <mergeCell ref="B54:B59"/>
+    <mergeCell ref="B61:B62"/>
+    <mergeCell ref="B98:B100"/>
+    <mergeCell ref="F123:F124"/>
+    <mergeCell ref="B117:B121"/>
+    <mergeCell ref="B84:B86"/>
+    <mergeCell ref="B87:B88"/>
     <mergeCell ref="B246:B254"/>
     <mergeCell ref="B146:B149"/>
     <mergeCell ref="B75:B78"/>
@@ -10829,51 +10881,6 @@
     <mergeCell ref="B101:B102"/>
     <mergeCell ref="B109:B113"/>
     <mergeCell ref="B90:B94"/>
-    <mergeCell ref="E123:E124"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="B24:B27"/>
-    <mergeCell ref="B66:B69"/>
-    <mergeCell ref="B63:B65"/>
-    <mergeCell ref="B54:B59"/>
-    <mergeCell ref="B61:B62"/>
-    <mergeCell ref="B98:B100"/>
-    <mergeCell ref="F123:F124"/>
-    <mergeCell ref="B117:B121"/>
-    <mergeCell ref="B84:B86"/>
-    <mergeCell ref="B87:B88"/>
-    <mergeCell ref="B164:B170"/>
-    <mergeCell ref="B151:B155"/>
-    <mergeCell ref="B156:B162"/>
-    <mergeCell ref="B142:B144"/>
-    <mergeCell ref="K13:K17"/>
-    <mergeCell ref="K18:K22"/>
-    <mergeCell ref="B14:B18"/>
-    <mergeCell ref="B19:B23"/>
-    <mergeCell ref="B47:B53"/>
-    <mergeCell ref="B41:B46"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="F31:F32"/>
-    <mergeCell ref="B33:B35"/>
-    <mergeCell ref="B37:B40"/>
-    <mergeCell ref="B73:B74"/>
-    <mergeCell ref="B70:B71"/>
-    <mergeCell ref="B201:B203"/>
-    <mergeCell ref="B228:B229"/>
-    <mergeCell ref="B220:B227"/>
-    <mergeCell ref="B195:B200"/>
-    <mergeCell ref="B172:B174"/>
-    <mergeCell ref="B175:B177"/>
-    <mergeCell ref="B178:B183"/>
-    <mergeCell ref="B184:B187"/>
-    <mergeCell ref="B188:B192"/>
-    <mergeCell ref="B240:B245"/>
-    <mergeCell ref="B237:B239"/>
-    <mergeCell ref="B230:B236"/>
-    <mergeCell ref="B210:B212"/>
-    <mergeCell ref="B204:B209"/>
-    <mergeCell ref="B213:B219"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>